<commit_message>
make time the same
</commit_message>
<xml_diff>
--- a/data/wang2020fecal/B data.xlsx
+++ b/data/wang2020fecal/B data.xlsx
@@ -1215,8 +1215,8 @@
   <sheetPr/>
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="2"/>
@@ -1835,7 +1835,7 @@
         <v>13</v>
       </c>
       <c r="B56">
-        <v>17.6255707762557</v>
+        <v>16.90123452</v>
       </c>
       <c r="C56">
         <v>36.4583333333333</v>
@@ -1846,7 +1846,7 @@
         <v>13</v>
       </c>
       <c r="B57">
-        <v>24.6575342465753</v>
+        <v>24.0575342465753</v>
       </c>
       <c r="C57">
         <v>40</v>

</xml_diff>